<commit_message>
Dodane pliki uzytkownikow, zaktualizowane
</commit_message>
<xml_diff>
--- a/MaterialyPomocnicze/Backlog.xlsx
+++ b/MaterialyPomocnicze/Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia\Systemy informatyczne\UsterkiMechaniczne\MaterialyPomocnicze\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935" activeTab="1"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
   <si>
     <t>Product Backlog (lista wymagań)</t>
   </si>
@@ -300,12 +295,33 @@
   </si>
   <si>
     <t>Małgorzata Motyczko</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>Do rozbudowania</t>
+  </si>
+  <si>
+    <t>Brak zabezpieczeń, trzeba dopisać blokady</t>
+  </si>
+  <si>
+    <t>Brak zabezpieczenia dla niepoprawnych danych</t>
+  </si>
+  <si>
+    <t>Sebastian Bachorczyk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -463,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,9 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -544,6 +557,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +634,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -644,10 +666,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -679,7 +700,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -855,11 +875,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -891,7 +911,7 @@
       <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="1">
@@ -908,7 +928,7 @@
       <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="1">
@@ -923,7 +943,7 @@
       <c r="B4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="1"/>
       <c r="F4" s="16" t="s">
         <v>22</v>
@@ -934,7 +954,7 @@
       <c r="B5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="1"/>
       <c r="F5" s="18" t="s">
         <v>24</v>
@@ -945,7 +965,7 @@
       <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="1"/>
       <c r="F6" s="15" t="s">
         <v>45</v>
@@ -956,9 +976,9 @@
       <c r="B7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="1"/>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>84</v>
       </c>
     </row>
@@ -967,7 +987,7 @@
       <c r="B8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:6">
@@ -975,7 +995,7 @@
       <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6">
@@ -983,7 +1003,7 @@
       <c r="B10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:6">
@@ -991,7 +1011,7 @@
       <c r="B11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:6">
@@ -999,7 +1019,7 @@
       <c r="B12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6">
@@ -1007,7 +1027,7 @@
       <c r="B13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6">
@@ -1015,7 +1035,7 @@
       <c r="B14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="31"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:6">
@@ -1023,7 +1043,7 @@
       <c r="B15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="31"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6">
@@ -1031,7 +1051,7 @@
       <c r="B16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="31"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4">
@@ -1039,7 +1059,7 @@
       <c r="B17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="31"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
@@ -1047,7 +1067,7 @@
       <c r="B18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4">
@@ -1055,7 +1075,7 @@
       <c r="B19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4">
@@ -1063,7 +1083,7 @@
       <c r="B20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
@@ -1071,7 +1091,7 @@
       <c r="B21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="31"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4">
@@ -1079,7 +1099,7 @@
       <c r="B22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4">
@@ -1087,7 +1107,7 @@
       <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="31"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4">
@@ -1095,7 +1115,7 @@
       <c r="B24" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="31"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4">
@@ -1103,12 +1123,12 @@
       <c r="B25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1"/>
-      <c r="C26" s="31"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4">
@@ -1116,7 +1136,7 @@
       <c r="B27" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4">
@@ -1124,22 +1144,22 @@
       <c r="B28" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="31"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
-      <c r="C29" s="31"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="30" t="s">
         <v>69</v>
       </c>
       <c r="D30" s="1">
@@ -1150,10 +1170,10 @@
       <c r="A31" s="1">
         <v>2</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="30" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="1">
@@ -1164,10 +1184,10 @@
       <c r="A32" s="1">
         <v>3</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D32" s="1">
@@ -1181,11 +1201,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1225,10 +1245,10 @@
       <c r="C2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -1323,7 +1343,7 @@
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="32" t="s">
         <v>89</v>
       </c>
       <c r="E10" s="9" t="s">
@@ -1335,12 +1355,12 @@
       <c r="G10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -1360,7 +1380,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A12" s="35"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="21" t="s">
         <v>61</v>
       </c>
@@ -1384,7 +1404,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A13" s="35"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="25" t="s">
         <v>62</v>
       </c>
@@ -1394,7 +1414,7 @@
       <c r="D13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>73</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -1402,13 +1422,13 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="3.75" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="29.25" customHeight="1">
@@ -1421,10 +1441,10 @@
       <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="37" t="s">
         <v>59</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -1439,10 +1459,10 @@
       <c r="C16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="37" t="s">
         <v>59</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -1457,8 +1477,8 @@
       <c r="C17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="G17" s="26" t="s">
+      <c r="D17" s="30"/>
+      <c r="G17" s="37" t="s">
         <v>59</v>
       </c>
       <c r="H17" s="6" t="s">
@@ -1473,9 +1493,21 @@
       <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="31"/>
-    </row>
-    <row r="19" spans="1:8" ht="28.5">
+      <c r="D18" s="30"/>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34.5" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="25" t="s">
         <v>72</v>
@@ -1483,7 +1515,19 @@
       <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="30"/>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="7"/>
@@ -1492,6 +1536,12 @@
       </c>
       <c r="C20" s="1" t="s">
         <v>92</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1508,7 +1558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Aktualizacja backlogu, burndown chart. Naprawa testu (calendar nie przechodzi)
</commit_message>
<xml_diff>
--- a/MaterialyPomocnicze/Backlog.xlsx
+++ b/MaterialyPomocnicze/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19110" windowHeight="7575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
   <si>
     <t>Product Backlog (lista wymagań)</t>
   </si>
@@ -306,9 +306,6 @@
     <t>2.6</t>
   </si>
   <si>
-    <t>Do rozbudowania</t>
-  </si>
-  <si>
     <t>Brak zabezpieczeń, trzeba dopisać blokady</t>
   </si>
   <si>
@@ -321,10 +318,49 @@
     <t>Interfejsy użytowników</t>
   </si>
   <si>
-    <t>Nie zrobione</t>
-  </si>
-  <si>
     <t>2.7</t>
+  </si>
+  <si>
+    <t>Story3</t>
+  </si>
+  <si>
+    <t>Podpiecie tabeli kalendarz i komunikacja z bazą danych</t>
+  </si>
+  <si>
+    <t>Testy pokrywające kod</t>
+  </si>
+  <si>
+    <t>Bogdał Kamila</t>
+  </si>
+  <si>
+    <t>Jeden nie przechodzi</t>
+  </si>
+  <si>
+    <t>Panel dodawania zleceń</t>
+  </si>
+  <si>
+    <t>Nie zaczęte</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Nie wszystkie</t>
+  </si>
+  <si>
+    <t>Uzupełnianie dni wolnych od pracy przez kierownika; pracownicy widzą swoje grafiki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stworzyć scenariusze testowe! Do poszczególnych przypadków testowych tworzyć scenariusz. Od różnych miejsc, opisać w którym miejscu zaczynamy scenariusz, gdzie kończymy. Kompletnie opisany przypadek. </t>
   </si>
 </sst>
 </file>
@@ -354,7 +390,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +514,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,22 +610,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1218,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1460,7 +1505,7 @@
       <c r="D15" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>59</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -1478,7 +1523,7 @@
       <c r="D16" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="34" t="s">
         <v>59</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -1494,7 +1539,10 @@
         <v>60</v>
       </c>
       <c r="D17" s="30"/>
-      <c r="G17" s="35" t="s">
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="34" t="s">
         <v>59</v>
       </c>
       <c r="H17" s="6" t="s">
@@ -1513,11 +1561,11 @@
       <c r="E18" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="F18" s="33" t="s">
         <v>96</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>93</v>
@@ -1533,12 +1581,12 @@
       </c>
       <c r="D19" s="30"/>
       <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="F19" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="34" t="s">
         <v>59</v>
       </c>
       <c r="H19" s="6" t="s">
@@ -1553,8 +1601,8 @@
       <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>96</v>
+      <c r="G20" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>95</v>
@@ -1563,16 +1611,99 @@
     <row r="21" spans="1:8">
       <c r="A21" s="7"/>
       <c r="B21" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G21" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="5.25" customHeight="1">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="H21" s="6" t="s">
+    </row>
+    <row r="24" spans="1:8" ht="42.75">
+      <c r="A24" s="39"/>
+      <c r="B24" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.5">
+      <c r="A25" s="39"/>
+      <c r="B25" s="25" t="s">
         <v>102</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="39"/>
+      <c r="B26" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="39"/>
+      <c r="B27" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="99.75">
+      <c r="B30" s="25" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodanie walidacji po stronie klienta dla dodawnia nowych pracowników Stworzenie interfejsu dla admina Dodanie regexow w panelu dod. nowych pracownikow na imię, nazwisko i hasło.
</commit_message>
<xml_diff>
--- a/MaterialyPomocnicze/Backlog.xlsx
+++ b/MaterialyPomocnicze/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Product Backlog (lista wymagań)</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Widzi wszystkie opcje z kazdego konta</t>
   </si>
   <si>
-    <t>Po wejściu na stronę jest panel logowania i wyniki leleżne od stanowiska</t>
-  </si>
-  <si>
     <t>Po zalogowaniu widzi 2 tryby</t>
   </si>
   <si>
@@ -333,15 +330,6 @@
     <t>Bogdał Kamila</t>
   </si>
   <si>
-    <t>Jeden nie przechodzi</t>
-  </si>
-  <si>
-    <t>Panel dodawania zleceń</t>
-  </si>
-  <si>
-    <t>Nie zaczęte</t>
-  </si>
-  <si>
     <t>2.9</t>
   </si>
   <si>
@@ -354,13 +342,52 @@
     <t>3.1</t>
   </si>
   <si>
-    <t>Nie wszystkie</t>
-  </si>
-  <si>
     <t>Uzupełnianie dni wolnych od pracy przez kierownika; pracownicy widzą swoje grafiki</t>
   </si>
   <si>
-    <t xml:space="preserve">Stworzyć scenariusze testowe! Do poszczególnych przypadków testowych tworzyć scenariusz. Od różnych miejsc, opisać w którym miejscu zaczynamy scenariusz, gdzie kończymy. Kompletnie opisany przypadek. </t>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>0.5h</t>
+  </si>
+  <si>
+    <t>Po wejściu na stronę jest panel logowania i wyniki zależne od stanowiska</t>
+  </si>
+  <si>
+    <t>Podział godzinowy pracy</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stworzenie interfejsów sekretarki i admina.  </t>
+  </si>
+  <si>
+    <t>Story 4 i 5</t>
+  </si>
+  <si>
+    <t>Dodanie panelu dodawania nowych klientów dla sekretarki, walidacja.</t>
+  </si>
+  <si>
+    <t>Stworzenie wyszukiwarki klientów po dowolnej danej dla sekretarki</t>
+  </si>
+  <si>
+    <t>Dodanie podziału godzinowego w kalendarzu admina</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>Walidacja po stronie klienta dla panelu dodawania użytkowników. Regex na imię i nazwisko i hasło przy dodawaniu nowych pracowników</t>
   </si>
 </sst>
 </file>
@@ -513,13 +540,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0DF5B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,7 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,18 +642,30 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,6 +675,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB0DF5B"/>
       <color rgb="FF9EE260"/>
       <color rgb="FFFFFF89"/>
     </mruColors>
@@ -939,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -952,16 +991,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -969,16 +1008,16 @@
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>90</v>
+      <c r="C2" s="29" t="s">
+        <v>89</v>
       </c>
       <c r="D2" s="1">
         <v>9</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -986,242 +1025,270 @@
       <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>69</v>
+      <c r="C3" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="D3" s="1">
         <v>9</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="1"/>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="1"/>
-      <c r="F6" s="15" t="s">
-        <v>45</v>
+      <c r="F6" s="14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
-      <c r="B9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="29" t="s">
+        <v>109</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1"/>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
-      <c r="B12" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
-      <c r="B13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="30"/>
+      <c r="B13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="29"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
-      <c r="B15" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
-      <c r="B17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="30"/>
+      <c r="B18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="29"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1"/>
-      <c r="B19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="30"/>
+      <c r="B19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="29"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1"/>
-      <c r="B20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="30"/>
+      <c r="B20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="29"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1"/>
-      <c r="B21" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="30"/>
+      <c r="B21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="29"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1"/>
-      <c r="B22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="30"/>
+      <c r="B22" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="29"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1"/>
-      <c r="B23" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="30"/>
+      <c r="B23" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="29"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1"/>
-      <c r="B24" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="30"/>
+      <c r="B24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="29"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1"/>
-      <c r="B25" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="30"/>
+      <c r="B25" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="29"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1"/>
-      <c r="C26" s="30"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="30"/>
+      <c r="A27" s="1">
+        <v>11</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="29"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1"/>
-      <c r="B28" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="30"/>
+      <c r="B28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="29"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
-      <c r="C29" s="30"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>69</v>
+      <c r="B30" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="D30" s="1">
         <v>10</v>
@@ -1231,11 +1298,11 @@
       <c r="A31" s="1">
         <v>2</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>82</v>
+      <c r="B31" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>81</v>
       </c>
       <c r="D31" s="1">
         <v>10</v>
@@ -1245,11 +1312,11 @@
       <c r="A32" s="1">
         <v>3</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>88</v>
       </c>
       <c r="D32" s="1">
         <v>10</v>
@@ -1263,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1283,16 +1350,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1303,11 +1370,11 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>54</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="1"/>
@@ -1398,318 +1465,405 @@
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="29" t="s">
-        <v>75</v>
+      <c r="H10" s="28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="49.5" customHeight="1">
       <c r="A11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="22" t="s">
-        <v>59</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="37.5" customHeight="1">
       <c r="A12" s="37"/>
-      <c r="B12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>60</v>
       </c>
+      <c r="C12" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>65</v>
       </c>
+      <c r="G12" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="H12" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30.75" customHeight="1">
       <c r="A13" s="37"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="3.75" customHeight="1">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="29.25" customHeight="1">
+      <c r="A15" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="3.75" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:8" ht="30" customHeight="1">
+      <c r="A16" s="40"/>
+      <c r="B16" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="34" t="s">
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.5">
+      <c r="A17" s="40"/>
+      <c r="B17" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="34" t="s">
+      <c r="D17" s="29"/>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="42.75">
+      <c r="A18" s="40"/>
+      <c r="B18" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="42.75">
-      <c r="A18" s="7"/>
-      <c r="B18" s="25" t="s">
+      <c r="D18" s="29"/>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34.5" customHeight="1">
+      <c r="A19" s="40"/>
+      <c r="B19" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="33" t="s">
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G19" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="34.5" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" t="s">
+    <row r="20" spans="1:8">
+      <c r="A20" s="40"/>
+      <c r="B20" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="40"/>
+      <c r="B21" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="5.25" customHeight="1">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42.75">
+      <c r="A24" s="41"/>
+      <c r="B24" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.5">
+      <c r="A25" s="41"/>
+      <c r="B25" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="41"/>
+      <c r="B26" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="41"/>
+      <c r="B27" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="7"/>
-      <c r="B20" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="7"/>
-      <c r="B21" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="5.25" customHeight="1">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="42.75">
-      <c r="A24" s="39"/>
-      <c r="B24" s="25" t="s">
+      <c r="G27" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="6" customHeight="1">
+      <c r="A28" s="34"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="34"/>
+    </row>
+    <row r="29" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A29" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="28.5">
-      <c r="A25" s="39"/>
-      <c r="B25" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="39"/>
-      <c r="B26" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="39"/>
-      <c r="B27" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="99.75">
-      <c r="B30" s="25" t="s">
+    </row>
+    <row r="30" spans="1:8" ht="28.5">
+      <c r="A30" s="42"/>
+      <c r="B30" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>114</v>
       </c>
     </row>
+    <row r="31" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A31" s="42"/>
+      <c r="B31" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="67.5" customHeight="1">
+      <c r="A32" s="42"/>
+      <c r="B32" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.5">
+      <c r="A33" s="42"/>
+      <c r="B33" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A29:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>